<commit_message>
added volume-col to pool ui & server
</commit_message>
<xml_diff>
--- a/data/pool_general.xlsx
+++ b/data/pool_general.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" iterateCount="1" concurrentCalc="0"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="21">
   <si>
     <t>Sample</t>
   </si>
@@ -56,12 +56,6 @@
     <t>my sample plate 2</t>
   </si>
   <si>
-    <t>96 Well Eppendorf TwinTec PCR</t>
-  </si>
-  <si>
-    <t>384 Well Biorad PCR</t>
-  </si>
-  <si>
     <t>notes3</t>
   </si>
   <si>
@@ -81,6 +75,21 @@
   </si>
   <si>
     <t>labware_type</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>"Volume" column is optional</t>
+  </si>
+  <si>
+    <t>volume of &lt;=0 is skipped</t>
+  </si>
+  <si>
+    <t>PCR Adapter 384 Well and 384 Well Biorad PCR</t>
+  </si>
+  <si>
+    <t>PCR Adapter 96 Well and 96 Well Eppendorf TwinTec PCR</t>
   </si>
 </sst>
 </file>
@@ -116,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,48 +405,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -446,23 +462,29 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -472,23 +494,29 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -498,23 +526,29 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -524,23 +558,29 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
+      <c r="D5" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
         <v>6</v>
       </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
       <c r="H5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -550,23 +590,29 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>10</v>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
       <c r="H6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -576,23 +622,29 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" t="s">
-        <v>10</v>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E7">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
       <c r="H7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -602,23 +654,29 @@
       <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E8">
         <v>12</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
       <c r="H8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -628,20 +686,26 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E9">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
       <c r="H9" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>